<commit_message>
AUTOMATION-85 CS Test cases (+5) после спринта 13.5
</commit_message>
<xml_diff>
--- a/src/test/resources/etalon/combinesheets/CS_006.xlsx
+++ b/src/test/resources/etalon/combinesheets/CS_006.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="555" windowWidth="27495" windowHeight="11445"/>
+    <workbookView xWindow="189" yWindow="497" windowWidth="32537" windowHeight="15403"/>
   </bookViews>
   <sheets>
-    <sheet name="Combined data" sheetId="4" r:id="rId1"/>
+    <sheet name="Combined data" sheetId="5" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="Range101">#REF!</definedName>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>Column1</t>
   </si>
@@ -53,6 +53,51 @@
   </si>
   <si>
     <t>Row5</t>
+  </si>
+  <si>
+    <t>133</t>
+  </si>
+  <si>
+    <t>277</t>
+  </si>
+  <si>
+    <t>421</t>
+  </si>
+  <si>
+    <t>565</t>
+  </si>
+  <si>
+    <t>709</t>
+  </si>
+  <si>
+    <t>1863</t>
+  </si>
+  <si>
+    <t>3007</t>
+  </si>
+  <si>
+    <t>4151</t>
+  </si>
+  <si>
+    <t>5295</t>
+  </si>
+  <si>
+    <t>10219</t>
+  </si>
+  <si>
+    <t>960.5</t>
+  </si>
+  <si>
+    <t>1464.5</t>
+  </si>
+  <si>
+    <t>1968.5</t>
+  </si>
+  <si>
+    <t>2472.5</t>
+  </si>
+  <si>
+    <t>11976.5</t>
   </si>
 </sst>
 </file>
@@ -69,18 +114,24 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
       <b/>
@@ -88,10 +139,14 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
       <sz val="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="7">
@@ -156,12 +211,12 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -379,13 +434,11 @@
   </sheetPr>
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -408,7 +461,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
@@ -427,13 +480,13 @@
       <c r="F2" s="6">
         <v>100</v>
       </c>
-      <c r="G2" s="7">
-        <v>133</v>
+      <c r="G2" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -452,13 +505,13 @@
       <c r="F3" s="6">
         <v>200</v>
       </c>
-      <c r="G3" s="7">
-        <v>277</v>
+      <c r="G3" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -477,13 +530,13 @@
       <c r="F4" s="6">
         <v>300</v>
       </c>
-      <c r="G4" s="7">
-        <v>421</v>
+      <c r="G4" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -502,13 +555,13 @@
       <c r="F5" s="6">
         <v>400</v>
       </c>
-      <c r="G5" s="7">
-        <v>565</v>
+      <c r="G5" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -527,139 +580,139 @@
       <c r="F6" s="6">
         <v>500</v>
       </c>
-      <c r="G6" s="7">
-        <v>709</v>
+      <c r="G6" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="10">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A7" s="14"/>
+      <c r="B7" s="9">
         <v>11</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="9">
         <v>22</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <v>310</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="9">
         <v>420</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="9">
         <v>1100</v>
       </c>
-      <c r="G7" s="11">
-        <v>1863</v>
-      </c>
-      <c r="H7" s="10" t="s">
+      <c r="G7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="9" t="s">
         <v>6</v>
       </c>
       <c r="I7" s="8"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="12">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A8" s="14"/>
+      <c r="B8" s="11">
         <v>13</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="11">
         <v>24</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="11">
         <v>330</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="11">
         <v>440</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="11">
         <v>2200</v>
       </c>
-      <c r="G8" s="13">
-        <v>3007</v>
-      </c>
-      <c r="H8" s="12" t="s">
+      <c r="G8" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="11" t="s">
         <v>7</v>
       </c>
       <c r="I8" s="8"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A9" s="14"/>
+      <c r="B9" s="9">
         <v>15</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="9">
         <v>26</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="9">
         <v>350</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="9">
         <v>460</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="9">
         <v>3300</v>
       </c>
-      <c r="G9" s="11">
-        <v>4151</v>
-      </c>
-      <c r="H9" s="10" t="s">
+      <c r="G9" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="9" t="s">
         <v>8</v>
       </c>
       <c r="I9" s="8"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="12">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A10" s="14"/>
+      <c r="B10" s="11">
         <v>17</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="11">
         <v>28</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="11">
         <v>370</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="11">
         <v>480</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="11">
         <v>4400</v>
       </c>
-      <c r="G10" s="13">
-        <v>5295</v>
-      </c>
-      <c r="H10" s="12" t="s">
+      <c r="G10" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="11" t="s">
         <v>9</v>
       </c>
       <c r="I10" s="8"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="10">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A11" s="14"/>
+      <c r="B11" s="9">
         <v>19</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="9">
         <v>210</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="9">
         <v>390</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="9">
         <v>4100</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="9">
         <v>5500</v>
       </c>
-      <c r="G11" s="11">
-        <v>10219</v>
-      </c>
-      <c r="H11" s="10" t="s">
+      <c r="G11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="9" t="s">
         <v>10</v>
       </c>
       <c r="I11" s="8"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A12" s="14"/>
       <c r="B12" s="6">
         <v>51</v>
       </c>
@@ -675,16 +728,16 @@
       <c r="F12" s="6">
         <v>600</v>
       </c>
-      <c r="G12" s="14">
-        <v>960.5</v>
-      </c>
-      <c r="H12" s="9"/>
+      <c r="G12" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="14"/>
       <c r="I12" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A13" s="14"/>
       <c r="B13" s="6">
         <v>53</v>
       </c>
@@ -700,16 +753,16 @@
       <c r="F13" s="6">
         <v>700</v>
       </c>
-      <c r="G13" s="14">
-        <v>1464.5</v>
-      </c>
-      <c r="H13" s="9"/>
+      <c r="G13" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="14"/>
       <c r="I13" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A14" s="14"/>
       <c r="B14" s="6">
         <v>55</v>
       </c>
@@ -725,16 +778,16 @@
       <c r="F14" s="6">
         <v>800</v>
       </c>
-      <c r="G14" s="14">
-        <v>1968.5</v>
-      </c>
-      <c r="H14" s="9"/>
+      <c r="G14" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" s="14"/>
       <c r="I14" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A15" s="14"/>
       <c r="B15" s="6">
         <v>57</v>
       </c>
@@ -750,16 +803,16 @@
       <c r="F15" s="6">
         <v>900</v>
       </c>
-      <c r="G15" s="14">
-        <v>2472.5</v>
-      </c>
-      <c r="H15" s="9"/>
+      <c r="G15" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="14"/>
       <c r="I15" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A16" s="14"/>
       <c r="B16" s="6">
         <v>59</v>
       </c>
@@ -775,10 +828,10 @@
       <c r="F16" s="6">
         <v>10000</v>
       </c>
-      <c r="G16" s="14">
-        <v>11976.5</v>
-      </c>
-      <c r="H16" s="9"/>
+      <c r="G16" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="14"/>
       <c r="I16" s="5" t="s">
         <v>10</v>
       </c>

</xml_diff>